<commit_message>
Add new set to track and new websites
</commit_message>
<xml_diff>
--- a/config_sets.xlsx
+++ b/config_sets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adl\Documents\Divers\Scripts Python\lego-price-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE76363-BE18-4EFC-898B-81AE0A96180A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCC5A1E-A159-4670-BB27-506FFFBB2FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ID_Set</t>
   </si>
@@ -44,40 +44,61 @@
     <t>Nom_Set</t>
   </si>
   <si>
-    <t>Site</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Selecteur</t>
-  </si>
-  <si>
-    <t>Amazon</t>
-  </si>
-  <si>
     <t>Bonsaï d’érable rouge du Japon</t>
   </si>
   <si>
-    <t>Lego.com</t>
-  </si>
-  <si>
-    <t>https://www.lego.com/fr-fr/product/japanese-red-maple-bonsai-tree-10348</t>
-  </si>
-  <si>
-    <t>standard</t>
-  </si>
-  <si>
-    <t>[data-test="product-price"]</t>
-  </si>
-  <si>
-    <t>amazon</t>
-  </si>
-  <si>
     <t>https://www.amazon.fr/dp/B0DWF6VKYB</t>
+  </si>
+  <si>
+    <t>URL_Amazon</t>
+  </si>
+  <si>
+    <t>URL_Auchan</t>
+  </si>
+  <si>
+    <t>URL_Leclerc</t>
+  </si>
+  <si>
+    <t>URL_Lego</t>
+  </si>
+  <si>
+    <t>https://www.auchan.fr/lego-botanicals-icons-10348-bonsai-d-erable-rouge-du-japon/pr-C1839443</t>
+  </si>
+  <si>
+    <t>https://www.e.leclerc/fp/lego-botanique-bonsai-d-erable-rouge-du-japon-decoration-vegetale-10348-5702017814674</t>
+  </si>
+  <si>
+    <t>La machine volante de Léonard de Vinci</t>
+  </si>
+  <si>
+    <t>Shelby Cobra 427 S/C</t>
+  </si>
+  <si>
+    <t>La planète Terre et la Lune en orbite</t>
+  </si>
+  <si>
+    <t>Mario Kart : Mario et kart standard</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/LEGO-10363-Icons/dp/B01NAELBNS</t>
+  </si>
+  <si>
+    <t>https://www.e.leclerc/fp/lego-icons-la-machine-volante-de-leonard-de-vinci-10363-5702017815893</t>
+  </si>
+  <si>
+    <t>https://www.auchan.fr/lego-icons-10363-machine-a-voler-leonardo-de-vinci/pr-C1825565</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/Technic-Building-Imaginative-Independent-Birthday/dp/B0DLZDDL1F</t>
+  </si>
+  <si>
+    <t>https://www.e.leclerc/fp/la-planete-terre-et-la-lune-en-orbite-5702017584133?srsltid=AfmBOop8NM1B7783jZYpdYv0gv5VSAZBW-RUnZOD-Y5-SxNFC-i5PgnG</t>
+  </si>
+  <si>
+    <t>https://www.auchan.fr/lego-lego-technic-42179-la-planete-terre-et-la-lune-en-orbite-jouet-theme-du-systeme-solaire/pr-C1769135</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/LEGO-Mario-Kart-Personnage-Construire/dp/B0DWM6NM4Y</t>
   </si>
 </sst>
 </file>
@@ -406,20 +427,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -430,16 +451,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -447,43 +468,98 @@
         <v>10348</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="str">
+        <f>_xlfn.CONCAT("https://www.lego.com/fr-fr/product/",A2)</f>
+        <v>https://www.lego.com/fr-fr/product/10348</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>10348</v>
+        <v>10363</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D6" si="0">_xlfn.CONCAT("https://www.lego.com/fr-fr/product/",A3)</f>
+        <v>https://www.lego.com/fr-fr/product/10363</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10357</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.lego.com/fr-fr/product/10357</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>42179</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.lego.com/fr-fr/product/42179</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>72037</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.lego.com/fr-fr/product/72037</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{A62C0F38-66F0-4EBB-85C9-0A2D96C334F6}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{9D44B775-EBC2-4AEB-A408-0D596EDE8707}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{A62C0F38-66F0-4EBB-85C9-0A2D96C334F6}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{017150D4-D8EE-48AE-84A0-D3F911D9E182}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{1D744576-95AB-4634-9F49-A0955F25CEF6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correction for Carrefour and code refactor
</commit_message>
<xml_diff>
--- a/config_sets.xlsx
+++ b/config_sets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adl\Documents\Divers\Scripts Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA70638-EFB0-4ED7-9EEA-CACDA457DD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EB0AF6-FB69-4074-84A1-9DA16965C996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -490,7 +490,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Automatically update sets from .txt files
</commit_message>
<xml_diff>
--- a/config_sets.xlsx
+++ b/config_sets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1111,6 +1111,157 @@
       </c>
       <c r="K14" t="inlineStr"/>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>43230</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>La caméra Hommage à Walt Disney</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>811</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Disney™</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://www.lego.com/cdn/cs/set/assets/blta0d2ef903df1c30c/43230.png?format=webply&amp;fit=bounds&amp;quality=75&amp;width=528&amp;height=528&amp;dpr=1</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://amzn.eu/d/b1S8pul</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>https://www.lego.com/fr-fr/product/43230</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>https://www.auchan.fr/lego-lego-disney-43230-la-camera-hommage-a-walt-disney-maquette-pour-adultes-avec-mickey-et-minnie-mouse/pr-C1718290</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>10368</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Le chrysanthème</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>278</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>The Botanical Collection</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>https://www.lego.com/cdn/cs/set/assets/bltdbc3129b50f61480/10368_Prod.png?format=webply&amp;fit=bounds&amp;quality=75&amp;width=528&amp;height=528&amp;dpr=1</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://amzn.eu/d/hoKJjfA</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>https://www.lego.com/fr-fr/product/10368</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>https://www.auchan.fr/lego-icons-10368-chrysantheme-collection-botanique/pr-C1802539</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>https://www.e.leclerc/fp/lego-icons-10368-le-chrysantheme-set-de-construction-5702017719689</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>https://www.carrefour.fr/p/lego-icons-le-chrysantheme-10368-lego-5702017719689</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>43257</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>784</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Disney™</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://www.lego.com/cdn/cs/set/assets/blt56c61562d64dc2e4/43257_Prod_en-gb.png?format=webply&amp;fit=bounds&amp;quality=75&amp;width=528&amp;height=528&amp;dpr=1</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://amzn.eu/d/eRPMY6r</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>https://www.lego.com/fr-fr/product/43257</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>https://www.auchan.fr/lego-disney-43257-angel-stitch/pr-C1836201</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>https://www.e.leclerc/fp/lego-disney-angel-jouet-de-construction-lilo-et-stitch-pour-filles-et-garcons-43257-5702017813967</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>https://www.carrefour.fr/p/lego-angel-43257-lego-5702017813967</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update price, config and deal data
</commit_message>
<xml_diff>
--- a/config_sets.xlsx
+++ b/config_sets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1497,6 +1497,114 @@
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>10796</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Nom non trouvé</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>165</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>https://www.lego.com/cdn/cs/set/assets/blt8ceb255a3e66c253/10796.png?format=webply&amp;fit=bounds&amp;quality=75&amp;width=528&amp;height=528&amp;dpr=1</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>https://www.lego.com/fr-fr/product/10796</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>77246</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Nom non trouvé</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>248</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>https://www.lego.com/cdn/cs/set/assets/blt0a45cbfbac56a36b/77246_Prod_en-gb.png?format=webply&amp;fit=bounds&amp;quality=75&amp;width=528&amp;height=528&amp;dpr=1</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>https://www.lego.com/fr-fr/product/77246</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>42154</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Nom non trouvé</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>1468</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>https://www.lego.com/cdn/cs/set/assets/blt5014244d8d8dc8ad/42154.png?format=webply&amp;fit=bounds&amp;quality=75&amp;width=528&amp;height=528&amp;dpr=1</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>https://www.lego.com/fr-fr/product/42154</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>